<commit_message>
dummy data to excel with styleing
</commit_message>
<xml_diff>
--- a/BlueBird/dumy.xlsx
+++ b/BlueBird/dumy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500"/>
+    <workbookView xWindow="33600" yWindow="-7300" windowWidth="51200" windowHeight="28300"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="279">
   <si>
     <t>2022년 04월분 급여지급명세서</t>
   </si>
@@ -124,6 +124,1201 @@
     <t xml:space="preserve">지급총계 
 공제총계 
 차인지급액</t>
+  </si>
+  <si>
+    <t xml:space="preserve">208
+이호완 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-10-13
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,122,000
+756
+34.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30.2
+27.5
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34
+7
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296,480
+14,000
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,030
+9,220
+2484</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,122,000
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">310,480
+1,173,734
+-863,254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">184
+신병만 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-02-17
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,346,600
+3147
+130.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">116.9
+114.4
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">133
+7
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,159,760
+14,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">605,970
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+37,120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,770
+6,620
+16151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,346,600
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,018,903
+4,435,261
+-2,416,358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">207
+석종현 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-10-01
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,396,300
+1774
+59.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.5
+64.5
+25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69
+7
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">601,680
+14,000
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,600
+4,740
+4925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,396,300
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">615,680
+2,426,565
+-1,810,885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">209
+여홍대 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-01-28
+6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,657,900
+3308
+130.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">125.3
+120.3
+26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">138
+6
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,203,360
+12,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+59,794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">746,055
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+48,870</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,900
+8,720
+18083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,657,900
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,260,382
+4,771,473
+-2,511,091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">212
+남재원 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-04-12
+5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,388,900
+2493
+99.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91.2
+90.6
+27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94
+5
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">819,680
+10,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175,005
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,360
+5,380
+9951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,388,900
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,243,858
+3,427,591
+-2,183,733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">217
+김태원 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-07-01
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,862,400
+1430
+52.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.1
+52
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57
+4
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497,040
+8,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,680
+7,060
+5954</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,862,400
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">744,213
+1,906,094
+-1,161,881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201
+류지봉 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-12-01
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47,900
+31
+0.57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3
+1.1
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
+4
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8,720
+8,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,790
+5,480
+2047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47,900
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255,893
+79,217
+176,676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">196
+박경식 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-09-01
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,185,000
+3288
+97.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85.7
+119.6
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111
+4
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">967,920
+8,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83,250
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36,050
+8,300
+10387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,185,000
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,298,343
+3,239,737
+-1,941,394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249
+우영조 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-03-01
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,329,800
+964
+52.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.8
+35.1
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45
+3
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">392,400
+6,000
+59,794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24,600
+5,660
+3666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,329,800
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">458,194
+1,363,726
+-905,532</t>
+  </si>
+  <si>
+    <t xml:space="preserve">193
+박진환 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01-01
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">856,900
+583
+26.33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.1
+21.2
+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26
+3
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">226,720
+6,000
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16,830
+3,860
+1862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">856,900
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232,720
+879,452
+-646,732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">221
+이유곤 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-03-21
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,302,100
+1568
+75.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61.9
+57
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71
+3
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">619,120
+6,000
+119,587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,500
+4,480
+5958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,302,100
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">744,707
+2,332,038
+-1,587,331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">224
+정석금 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-22
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,987,700
+1467
+50.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.5
+53.4
+26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58
+3
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">505,760
+6,000
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+18,940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,700
+3,380
+4094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,987,700
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511,760
+2,028,814
+-1,517,054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246
+최철은 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11-05
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711,300
+520
+24.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.1
+18.9
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23
+3
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200,560
+6,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49,360
+11,360
+3566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">711,300
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445,733
+775,586
+-329,853</t>
+  </si>
+  <si>
+    <t xml:space="preserve">186
+이호준 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01-24
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,908,300
+2182
+83.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.2
+79.3
+27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80
+3
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">697,600
+6,000
+179,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,260
+5,800
+7064</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,908,300
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">882,980
+2,946,424
+-2,063,444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">199
+정길호 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01-25
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,932,800
+2266
+83.53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.9
+82.4
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82
+3
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">715,040
+6,000
+119,587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+24,880</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19,300
+4,440
+6725</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,932,800
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">840,627
+2,988,145
+-2,147,518</t>
+  </si>
+  <si>
+    <t xml:space="preserve">225
+서헌교 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-09-04
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,055,600
+2445
+101.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.2
+88.9
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91
+3
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">793,520
+6,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,020
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,010
+5,980
+8510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,055,600
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,063,713
+3,096,100
+-2,032,387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200
+권동역 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-04-01
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,261,100
+2652
+113.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87.7
+96.4
+24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109
+3
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">950,480
+6,000
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">117,495
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26,550
+6,100
+10505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,261,100
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,313,148
+3,304,255
+-1,991,107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198
+이승주 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-10-24
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,496,700
+2813
+91.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94.1
+102.3
+28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96
+3
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">837,120
+6,000
+179,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">223,515
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+28,980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22,490
+5,180
+9968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,496,700
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,246,015
+3,563,318
+-2,317,303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232
+박무준 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-03-01
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,001,500
+2480
+87.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.7
+90.2
+28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86
+2
+3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">749,920
+4,000
+179,380</t>
+  </si>
+  <si>
+    <t xml:space="preserve">675
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+32,800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,440
+5,860
+7472</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,001,500
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">933,975
+3,073,072
+-2,139,097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240
+안구혁 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-10-30
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,090,900
+875
+32.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.3
+31.8
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34
+2
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296,480
+4,000
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+42,120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32,640
+7,520
+2404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,090,900
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300,480
+1,175,584
+-875,104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">241
+황선식 
+정규기사</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-11-27
+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,411,700
+1845
+74.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.9
+67.1
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76
+2
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">662,720
+4,000
+59,794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+27,990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21,690
+4,980
+5812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,411,700
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">726,514
+2,472,172
+-1,745,658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4597
+하문수 
+null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-10-01
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,278,100
+3215
+112.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115.1
+116.9
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126
+0
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,098,720
+0
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">575,145
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+15304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,278,100
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,913,038
+4,293,404
+-2,380,366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15
+강찬수 
+null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,193,200
+5393
+199.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">193.5
+196.1
+27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216
+0
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,883,520
+0
+239,173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,886,940
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0
+0
+32077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,193,200
+0
+0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,009,633
+7,225,277
+-3,215,644</t>
   </si>
 </sst>
 </file>
@@ -546,16 +1741,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0" zoomScale="103" zoomScaleNormal="100">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0" defaultColWidth="8.83203125" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="10" width="7.83203125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
     <col min="11" max="12" width="12.83203125" customWidth="1"/>
     <col min="13" max="17" width="14.83203125" customWidth="1"/>
   </cols>
@@ -714,7 +1913,7 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -739,11 +1938,11 @@
       <c r="I8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="7" t="s">
         <v>24</v>
       </c>
@@ -758,6 +1957,1179 @@
       </c>
       <c r="Q8" s="7" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="9" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>12</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>15</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>16</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>17</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>18</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="27" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>19</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>20</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>21</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>22</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" ht="57" customHeight="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>23</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>